<commit_message>
New Analysis and function to grab a ~50 dimensional matrix of all counts and phases
</commit_message>
<xml_diff>
--- a/FatMothSet1Guide.xlsx
+++ b/FatMothSet1Guide.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr/>
+  <workbookPr date1904="0"/>
+  <workbookProtection/>
   <bookViews>
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
   </extLst>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -39,64 +40,116 @@
     <t>pct_body</t>
   </si>
   <si>
+    <t>n_trials</t>
+  </si>
+  <si>
+    <t>fed_per_trial</t>
+  </si>
+  <si>
     <t>Tracking</t>
   </si>
   <si>
-    <t>Trials_Used</t>
-  </si>
-  <si>
-    <t>start_points</t>
+    <t>trial_pre</t>
+  </si>
+  <si>
+    <t>trial_post</t>
+  </si>
+  <si>
+    <t>start_pre</t>
+  </si>
+  <si>
+    <t>start_post</t>
+  </si>
+  <si>
+    <t>num_trials_fed</t>
+  </si>
+  <si>
+    <t>true_fed</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
+    <t>2024_10_28</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>[1,2]</t>
-  </si>
-  <si>
-    <t>[1,123000]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pulled Out many Wires, Have DLMs Rax RBa, LDVM, Only 2 trials of feeding</t>
   </si>
   <si>
-    <t>[]</t>
+    <t>2024_10_29</t>
   </si>
   <si>
     <t xml:space="preserve">Lost lsa, only bouts of flapping, okay tracking for first trail, no 10 seconds post feeding</t>
   </si>
   <si>
+    <t>2024_10_30</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lost LSA lol, bouts but never for 10 seconds post the first trial</t>
   </si>
   <si>
+    <t>2024_10_31</t>
+  </si>
+  <si>
     <t xml:space="preserve">Did not feed much, seemed to be responding hella to the flower during a non feeding post trial but was not tracking</t>
   </si>
   <si>
-    <t>[2,4]</t>
-  </si>
-  <si>
-    <t>[160000,1]</t>
+    <t>2024_11_01</t>
   </si>
   <si>
     <t xml:space="preserve">Took a while to get going but great feeding tracking and muscle signals, may have to re sort some stuff but good golly is this data nice</t>
+  </si>
+  <si>
+    <t>2024_11_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let it sit for a while, lost lsa, okay tracking</t>
+  </si>
+  <si>
+    <t>2024_11_05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Again sits for a while, all muscles, clean data</t>
+  </si>
+  <si>
+    <t>2024_11_07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">looks good, not too much feeding tho, its proboscis was kinda bent and mangled </t>
+  </si>
+  <si>
+    <t>2024_11_08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proboscis split in two but it still fed wow</t>
+  </si>
+  <si>
+    <t>2024_11_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lost the RSA, Tracking good esp at low frequencies </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,20 +169,46 @@
       <diagonal style="none"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+  <cellStyleXfs count="6">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -425,9 +504,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="">
+    <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
@@ -435,46 +514,46 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="18A303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="0369A3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A33E03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="8E03A3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="C99C00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="C9211E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0000EE"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="551A8B"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="">
@@ -482,71 +561,25 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -583,10 +616,10 @@
           <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -597,26 +630,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr filterMode="0">
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" zoomScale="100" workbookViewId="0">
+      <selection activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.6796875" defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="11.00390625"/>
-    <col bestFit="1" min="2" max="2" width="4.97265625"/>
-    <col bestFit="1" min="3" max="3" width="5.15234375"/>
-    <col bestFit="1" min="4" max="4" width="11.23046875"/>
-    <col bestFit="1" min="5" max="5" width="12.140625"/>
-    <col bestFit="1" min="6" max="6" width="5.61328125"/>
-    <col bestFit="1" min="7" max="7" width="8.69140625"/>
-    <col bestFit="1" min="8" max="8" width="7.8828125"/>
-    <col bestFit="1" min="10" max="10" width="11.05078125"/>
-    <col customWidth="1" min="11" max="11" width="70.7109375"/>
+    <col customWidth="1" min="1" max="1" style="0" width="11"/>
+    <col customWidth="1" min="2" max="2" style="0" width="4.9699999999999998"/>
+    <col customWidth="1" min="3" max="3" style="0" width="5.1500000000000004"/>
+    <col customWidth="1" min="4" max="4" style="0" width="11.24"/>
+    <col customWidth="1" min="5" max="5" style="0" width="12.15"/>
+    <col customWidth="1" min="6" max="6" style="0" width="5.6100000000000003"/>
+    <col customWidth="1" min="7" max="7" style="0" width="8.6899999999999995"/>
+    <col customWidth="1" min="8" max="8" style="0" width="7.8799999999999999"/>
+    <col bestFit="1" min="9" max="9" width="11.82421875"/>
+    <col bestFit="1" customWidth="1" min="10" max="10" style="0" width="7.953125"/>
+    <col bestFit="1" customWidth="1" min="11" max="11" style="0" width="8.08203125"/>
+    <col bestFit="1" min="12" max="12" width="8.90234375"/>
+    <col bestFit="1" customWidth="1" min="13" max="13" width="8.58203125"/>
+    <col bestFit="1" min="14" max="14" width="9.4140625"/>
+    <col customWidth="1" min="15" max="15" width="13.57421875"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="14.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -638,7 +680,7 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
@@ -650,124 +692,205 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" ht="14">
-      <c r="A2" s="1">
-        <v>45593</v>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3">
         <v>1.75</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2">
         <v>4.0949999999999998</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2">
         <v>3.512</v>
       </c>
       <c r="F2" s="4">
         <f t="shared" ref="F2:F9" si="0">D2-E2</f>
-        <v>0.58299999999999974</v>
-      </c>
-      <c r="G2" s="2">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="G2" s="3">
         <f t="shared" ref="G2:G9" si="1">F2/C2*100</f>
         <v>33.314285714285703</v>
       </c>
       <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" ht="14">
-      <c r="A3" s="1">
-        <v>45594</v>
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <f>G2/H2</f>
+        <v>16.657142857142851</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>(L2+((N2+(5*10^4))/(3*10^5))-(K2+((M2+(5*10^4))/(3*10^5))))</f>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <f>O2*I2</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3">
+        <v>18</v>
+      </c>
+      <c r="C3">
         <v>1.6100000000000001</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3">
         <v>4.6769999999999996</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>3.9430000000000001</v>
       </c>
       <c r="F3" s="4">
         <f t="shared" si="0"/>
-        <v>0.73399999999999954</v>
-      </c>
-      <c r="G3" s="2">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="G3" s="3">
         <f t="shared" si="1"/>
-        <v>45.59006211180121</v>
+        <v>45.590062111801203</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>45595</v>
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <f>G3/H3</f>
+        <v>11.397515527950301</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>(L3+((N3+(5*10^4))/(3*10^5))-(K3+((M3+(5*10^4))/(3*10^5))))</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f>O3*I3</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3">
         <v>1.49</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4">
         <v>4.4340000000000002</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4">
         <v>3.726</v>
       </c>
       <c r="F4" s="4">
         <f t="shared" si="0"/>
-        <v>0.70800000000000018</v>
-      </c>
-      <c r="G4" s="2">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="G4" s="3">
         <f t="shared" si="1"/>
-        <v>47.516778523489947</v>
+        <v>47.516778523489997</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" ht="68.650000000000006" customHeight="1">
-      <c r="A5" s="1">
-        <v>45596</v>
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <f>G4/H4</f>
+        <v>11.879194630872499</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>(L4+((N4+(5*10^4))/(3*10^5))-(K4+((M4+(5*10^4))/(3*10^5))))</f>
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f>O4*I4</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" ht="14">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>2.1099999999999999</v>
@@ -780,31 +903,52 @@
       </c>
       <c r="F5" s="4">
         <f t="shared" si="0"/>
-        <v>0.15599999999999969</v>
-      </c>
-      <c r="G5" s="2">
+        <v>0.156</v>
+      </c>
+      <c r="G5" s="3">
         <f t="shared" si="1"/>
-        <v>7.3933649289099383</v>
+        <v>7.3933649289099401</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <f>G5/H5</f>
+        <v>3.6966824644549701</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>(L5+((N5+(5*10^4))/(3*10^5))-(K5+((M5+(5*10^4))/(3*10^5))))</f>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <f>O5*I5</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25">
-      <c r="A6" s="5">
-        <v>45597</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
       <c r="C6">
         <v>1.75</v>
@@ -817,73 +961,334 @@
       </c>
       <c r="F6" s="4">
         <f t="shared" si="0"/>
-        <v>0.43399999999999972</v>
-      </c>
-      <c r="G6" s="2">
+        <v>0.434</v>
+      </c>
+      <c r="G6" s="3">
         <f t="shared" si="1"/>
-        <v>24.799999999999983</v>
+        <v>24.800000000000001</v>
       </c>
       <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" t="s">
-        <v>21</v>
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <f>G6/H6</f>
+        <v>6.2000000000000002</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>150000</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <f>(L6+((N6+(5*10^4))/(3*10^5))-(K6+((M6+(5*10^4))/(3*10^5))))</f>
+        <v>1.5000033333333334</v>
+      </c>
+      <c r="P6">
+        <f>O6*I6</f>
+        <v>9.3000206666666667</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" ht="14.25">
+      <c r="A7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="D7">
+        <v>4.4660000000000002</v>
+      </c>
+      <c r="E7">
+        <v>4.0940000000000003</v>
+      </c>
       <c r="F7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="e">
+        <v>0.372</v>
+      </c>
+      <c r="G7" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>18.507462686567202</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <f>G7/H7</f>
+        <v>4.6268656716418004</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>150000</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <f>(L7+((N7+(5*10^4))/(3*10^5))-(K7+((M7+(5*10^4))/(3*10^5))))</f>
+        <v>1.5000033333333334</v>
+      </c>
+      <c r="P7">
+        <f>O7*I7</f>
+        <v>6.9403139303482728</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" ht="14.25">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>2.1899999999999999</v>
+      </c>
+      <c r="D8">
+        <v>4.8310000000000004</v>
+      </c>
+      <c r="E8">
+        <v>4.3479999999999999</v>
+      </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="2" t="e">
+        <v>0.48300000000000054</v>
+      </c>
+      <c r="G8" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>22.054794520547972</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <f>G8/H8</f>
+        <v>5.513698630136993</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8" s="6">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>100000</v>
+      </c>
+      <c r="O8">
+        <f>(L8+((N8+(5*10^4))/(3*10^5))-(K8+((M8+(5*10^4))/(3*10^5))))</f>
+        <v>3.3333300000000001</v>
+      </c>
+      <c r="P8">
+        <f>O8*I8</f>
+        <v>18.378977054794543</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" ht="14.25">
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>1.8</v>
+      </c>
+      <c r="D9">
+        <v>4.8010000000000002</v>
+      </c>
+      <c r="E9">
+        <v>4.6369999999999996</v>
+      </c>
       <c r="F9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="2" t="e">
+        <v>0.16400000000000059</v>
+      </c>
+      <c r="G9" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>9.1111111111111427</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <f>G9/H9</f>
+        <v>2.2777777777777857</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9" s="6">
+        <v>10000</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <f>(L9+((N9+(5*10^4))/(3*10^5))-(K9+((M9+(5*10^4))/(3*10^5))))</f>
+        <v>1.9666699999999999</v>
+      </c>
+      <c r="P9">
+        <f>O9*I9</f>
+        <v>4.4796372222222374</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" ht="14.25">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>1.79</v>
+      </c>
+      <c r="D10">
+        <v>4.5369999999999999</v>
+      </c>
+      <c r="E10">
+        <v>3.7650000000000001</v>
+      </c>
       <c r="F10" s="4">
         <f t="shared" ref="F10:F19" si="2">D10-E10</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="2" t="e">
+        <v>0.7719999999999998</v>
+      </c>
+      <c r="G10" s="3">
         <f t="shared" ref="G10:G19" si="3">F10/C10*100</f>
-        <v>#DIV/0!</v>
+        <v>43.128491620111717</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <f>G10/H10</f>
+        <v>10.782122905027929</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10" s="6">
+        <v>100000</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <f>(L10+((N10+(5*10^4))/(3*10^5))-(K10+((M10+(5*10^4))/(3*10^5))))</f>
+        <v>1.6666699999999999</v>
+      </c>
+      <c r="P10">
+        <f>O10*I10</f>
+        <v>17.970240782122897</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" ht="14.25">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>1.8100000000000001</v>
+      </c>
+      <c r="D11">
+        <v>3.9510000000000001</v>
+      </c>
+      <c r="E11">
+        <v>3.391</v>
+      </c>
       <c r="F11" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="2" t="e">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G11" s="3">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>30.939226519337019</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <f>G11/H11</f>
+        <v>15.46961325966851</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11" s="6">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <f>(L11+((N11+(5*10^4))/(3*10^5))-(K11+((M11+(5*10^4))/(3*10^5))))</f>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="P11">
+        <f>O11*I11</f>
+        <v>15.469613259668506</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" ht="14.25">
@@ -891,8 +1296,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G12" s="2" t="e">
+      <c r="G12" s="3" t="e">
         <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I12" t="e">
+        <f>G12/H12</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -901,8 +1310,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G13" s="2" t="e">
+      <c r="G13" s="3" t="e">
         <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" t="e">
+        <f>G13/H13</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -911,8 +1324,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G14" s="2" t="e">
+      <c r="G14" s="3" t="e">
         <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" t="e">
+        <f>G14/H14</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -921,8 +1338,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G15" s="2" t="e">
+      <c r="G15" s="3" t="e">
         <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" t="e">
+        <f>G15/H15</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -931,8 +1352,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G16" s="2" t="e">
+      <c r="G16" s="3" t="e">
         <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" t="e">
+        <f>G16/H16</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -941,8 +1366,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G17" s="2" t="e">
+      <c r="G17" s="3" t="e">
         <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" t="e">
+        <f>G17/H17</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -951,8 +1380,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G18" s="2" t="e">
+      <c r="G18" s="3" t="e">
         <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" t="e">
+        <f>G18/H18</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -961,15 +1394,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G19" s="2" t="e">
+      <c r="G19" s="3" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="I19" t="e">
+        <f>G19/H19</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="J24" s="6"/>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <printOptions headings="0" gridLines="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins left="0.70069444444444484" right="0.70069444444444484" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51181102362204689" footer="0.51181102362204689"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SICB Push WOOHOO More moths More analysis of coordinated muscle activity
</commit_message>
<xml_diff>
--- a/FatMothSet1Guide.xlsx
+++ b/FatMothSet1Guide.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -140,6 +140,39 @@
   </si>
   <si>
     <t xml:space="preserve">Great Data Tbh</t>
+  </si>
+  <si>
+    <t>2024_11_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Great Tracking, Lost A lot of wires so dont use it</t>
+  </si>
+  <si>
+    <t>2024_12_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meh behavior</t>
+  </si>
+  <si>
+    <t>2024_08_01</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>COLD!</t>
+  </si>
+  <si>
+    <t>2024_06_06</t>
+  </si>
+  <si>
+    <t>2024_06_20</t>
+  </si>
+  <si>
+    <t>Cold!</t>
+  </si>
+  <si>
+    <t>2024_06_24</t>
   </si>
 </sst>
 </file>
@@ -161,12 +194,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -188,7 +227,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -204,7 +243,25 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyProtection="0">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
@@ -644,14 +701,14 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" topLeftCell="D1" zoomScale="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" topLeftCell="G1" zoomScale="100" workbookViewId="0">
       <selection activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6796875" defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" style="0" width="11"/>
-    <col customWidth="1" min="2" max="2" style="0" width="4.9699999999999998"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="0" width="6.87109375"/>
     <col customWidth="1" min="3" max="3" style="0" width="5.1500000000000004"/>
     <col customWidth="1" min="4" max="4" style="0" width="11.24"/>
     <col customWidth="1" min="5" max="5" style="0" width="12.15"/>
@@ -752,12 +809,14 @@
         <v>2</v>
       </c>
       <c r="I2">
-        <f>F2/H2</f>
+        <f t="shared" ref="I2:I9" si="2">F2/H2</f>
         <v>0.29149999999999998</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
       <c r="Q2" s="3"/>
       <c r="T2" t="s">
         <v>20</v>
@@ -791,12 +850,14 @@
         <v>4</v>
       </c>
       <c r="I3">
-        <f>F3/H3</f>
+        <f t="shared" si="2"/>
         <v>0.1835</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
       <c r="Q3" s="3"/>
       <c r="T3" t="s">
         <v>22</v>
@@ -830,12 +891,14 @@
         <v>4</v>
       </c>
       <c r="I4">
-        <f>F4/H4</f>
+        <f t="shared" si="2"/>
         <v>0.17699999999999999</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
       <c r="Q4" s="3"/>
       <c r="T4" t="s">
         <v>24</v>
@@ -869,644 +932,1354 @@
         <v>2</v>
       </c>
       <c r="I5">
-        <f>F5/H5</f>
+        <f t="shared" si="2"/>
         <v>0.078</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
       <c r="Q5" s="3"/>
       <c r="T5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" ht="14.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" s="6" customFormat="1" ht="14.25">
+      <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>1.75</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>4.2729999999999997</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>3.839</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="8">
         <f t="shared" si="0"/>
         <v>0.434</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="9">
         <f t="shared" si="1"/>
         <v>24.800000000000001</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="6">
         <v>4</v>
       </c>
-      <c r="I6">
-        <f>F6/H6</f>
+      <c r="I6" s="6">
+        <f t="shared" si="2"/>
         <v>0.1085</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
+      <c r="J6" s="6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6">
         <v>2</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="6">
         <v>4</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="10">
         <v>150000</v>
       </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="3">
-        <f>K6-1+(M6/(3*10^5))</f>
+      <c r="N6" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="9">
+        <f t="shared" ref="Q6:Q9" si="3">K6-1+(M6/(3*10^5))</f>
         <v>1.5</v>
       </c>
-      <c r="R6">
-        <f>C6+(Q6*I6)</f>
+      <c r="R6" s="6">
+        <f t="shared" ref="R6:R9" si="4">C6+(Q6*I6)</f>
         <v>1.91275</v>
       </c>
-      <c r="S6">
-        <f>R6+(O6*I6)</f>
+      <c r="S6" s="6">
+        <f t="shared" ref="S6:S9" si="5">R6+(O6*I6)</f>
         <v>1.91275</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" ht="14.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" s="6" customFormat="1" ht="14.25">
+      <c r="A7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>2.0099999999999998</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>4.4660000000000002</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>4.0940000000000003</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="8">
         <f t="shared" si="0"/>
         <v>0.372</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="9">
         <f t="shared" si="1"/>
         <v>18.507462686567202</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
         <v>4</v>
       </c>
-      <c r="I7">
-        <f>F7/H7</f>
+      <c r="I7" s="6">
+        <f t="shared" si="2"/>
         <v>0.092999999999999999</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
+      <c r="J7" s="6">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6">
         <v>2</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="6">
         <v>4</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="10">
         <v>150000</v>
       </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="3">
-        <f>K7-1+(M7/(3*10^5))</f>
+      <c r="N7" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="9">
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
-      <c r="R7">
-        <f>C7+(Q7*I7)</f>
+      <c r="R7" s="6">
+        <f t="shared" si="4"/>
         <v>2.1494999999999997</v>
       </c>
-      <c r="S7">
-        <f>R7+(O7*I7)</f>
+      <c r="S7" s="6">
+        <f t="shared" si="5"/>
         <v>2.1494999999999997</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" ht="14.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" s="6" customFormat="1" ht="14.25">
+      <c r="A8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>2.1899999999999999</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>4.8310000000000004</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <v>4.3479999999999999</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="8">
         <f t="shared" si="0"/>
         <v>0.48300000000000054</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="9">
         <f t="shared" si="1"/>
         <v>22.054794520547972</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="6">
         <v>4</v>
       </c>
-      <c r="I8">
-        <f>F8/H8</f>
+      <c r="I8" s="6">
+        <f t="shared" si="2"/>
         <v>0.12075000000000014</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
+      <c r="J8" s="6">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6">
+        <v>1</v>
+      </c>
+      <c r="L8" s="6">
         <v>4</v>
       </c>
-      <c r="M8" s="1">
-        <v>1</v>
-      </c>
-      <c r="N8">
+      <c r="M8" s="10">
+        <v>1</v>
+      </c>
+      <c r="N8" s="10">
         <v>100000</v>
       </c>
-      <c r="P8">
-        <f t="shared" ref="P8:P9" si="2">O8*I8</f>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="3">
-        <f>K8-1+(M8/(3*10^5))</f>
+      <c r="P8" s="6">
+        <f t="shared" ref="P8:P9" si="6">O8*I8</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="9">
+        <f t="shared" si="3"/>
         <v>3.3333333333333333e-06</v>
       </c>
-      <c r="R8">
-        <f>C8+(Q8*I8)</f>
+      <c r="R8" s="6">
+        <f t="shared" si="4"/>
         <v>2.1900004024999999</v>
       </c>
-      <c r="S8">
-        <f>R8+(O8*I8)</f>
+      <c r="S8" s="6">
+        <f t="shared" si="5"/>
         <v>2.1900004024999999</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="T8" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" s="6" customFormat="1" ht="14.25">
+      <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>1.8</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>4.8010000000000002</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>4.6369999999999996</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="8">
         <f t="shared" si="0"/>
         <v>0.16400000000000059</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="9">
         <f t="shared" si="1"/>
         <v>9.1111111111111427</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="6">
         <v>4</v>
       </c>
-      <c r="I9">
-        <f>F9/H9</f>
+      <c r="I9" s="6">
+        <f t="shared" si="2"/>
         <v>0.041000000000000147</v>
       </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
+      <c r="J9" s="6">
+        <v>1</v>
+      </c>
+      <c r="K9" s="6">
+        <v>1</v>
+      </c>
+      <c r="L9" s="6">
         <v>3</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="10">
         <v>10000</v>
       </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9">
+      <c r="N9" s="10">
+        <v>1</v>
+      </c>
+      <c r="O9" s="6">
         <f>(L9+((N9+(5*10^4))/(3*10^5))-(K9+((M9+(5*10^4))/(3*10^5))))</f>
         <v>1.9666699999999999</v>
       </c>
-      <c r="P9">
-        <f t="shared" si="2"/>
+      <c r="P9" s="6">
+        <f t="shared" si="6"/>
         <v>0.08063347000000029</v>
       </c>
-      <c r="Q9" s="3">
-        <f>K9-1+(M9/(3*10^5))</f>
+      <c r="Q9" s="9">
+        <f t="shared" si="3"/>
         <v>0.033333333333333333</v>
       </c>
-      <c r="R9">
-        <f>C9+(Q9*I9)</f>
+      <c r="R9" s="6">
+        <f t="shared" si="4"/>
         <v>1.8013666666666668</v>
       </c>
-      <c r="S9">
-        <f>R9+(O9*I9)</f>
+      <c r="S9" s="6">
+        <f t="shared" si="5"/>
         <v>1.882000136666667</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="T9" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" ht="14.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" s="6" customFormat="1" ht="14.25">
+      <c r="A10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>1.79</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>4.5369999999999999</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>3.7650000000000001</v>
       </c>
-      <c r="F10" s="4">
-        <f t="shared" ref="F10:F19" si="3">D10-E10</f>
+      <c r="F10" s="8">
+        <f t="shared" ref="F10:F32" si="7">D10-E10</f>
         <v>0.7719999999999998</v>
       </c>
-      <c r="G10" s="3">
-        <f t="shared" ref="G10:G19" si="4">F10/C10*100</f>
+      <c r="G10" s="9">
+        <f t="shared" ref="G10:G32" si="8">F10/C10*100</f>
         <v>43.128491620111717</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="6">
         <v>4</v>
       </c>
-      <c r="I10">
-        <f>F10/H10</f>
+      <c r="I10" s="6">
+        <f t="shared" ref="I10:I32" si="9">F10/H10</f>
         <v>0.19299999999999995</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
+      <c r="J10" s="6">
+        <v>1</v>
+      </c>
+      <c r="K10" s="6">
         <v>2</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="6">
         <v>4</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="10">
         <v>100000</v>
       </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <f t="shared" ref="O10:O11" si="5">(L10+((N10+(5*10^4))/(3*10^5))-(K10+((M10+(5*10^4))/(3*10^5))))</f>
+      <c r="N10" s="10">
+        <v>1</v>
+      </c>
+      <c r="O10" s="6">
+        <f t="shared" ref="O10:O26" si="10">(L10+((N10+(5*10^4))/(3*10^5))-(K10+((M10+(5*10^4))/(3*10^5))))</f>
         <v>1.6666699999999999</v>
       </c>
-      <c r="P10">
-        <f t="shared" ref="P10:P11" si="6">O10*I10</f>
+      <c r="P10" s="6">
+        <f t="shared" ref="P10:P30" si="11">O10*I10</f>
         <v>0.32166730999999987</v>
       </c>
-      <c r="Q10" s="3">
-        <f>K10-1+(M10/(3*10^5))</f>
+      <c r="Q10" s="9">
+        <f t="shared" ref="Q10:Q30" si="12">K10-1+(M10/(3*10^5))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="R10">
-        <f>C10+(Q10*I10)</f>
+      <c r="R10" s="6">
+        <f t="shared" ref="R10:R30" si="13">C10+(Q10*I10)</f>
         <v>2.0473333333333334</v>
       </c>
-      <c r="S10">
-        <f>R10+(O10*I10)</f>
+      <c r="S10" s="6">
+        <f t="shared" ref="S10:S30" si="14">R10+(O10*I10)</f>
         <v>2.3690006433333335</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="T10" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" ht="14.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" s="6" customFormat="1" ht="14.25">
+      <c r="A11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>1.8100000000000001</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>3.9510000000000001</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
         <v>3.391</v>
       </c>
-      <c r="F11" s="4">
-        <f t="shared" si="3"/>
+      <c r="F11" s="8">
+        <f t="shared" si="7"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="G11" s="3">
-        <f t="shared" si="4"/>
+      <c r="G11" s="9">
+        <f t="shared" si="8"/>
         <v>30.939226519337019</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="6">
         <v>2</v>
       </c>
-      <c r="I11">
-        <f>F11/H11</f>
+      <c r="I11" s="6">
+        <f t="shared" si="9"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
+      <c r="J11" s="6">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1</v>
+      </c>
+      <c r="L11" s="6">
         <v>2</v>
       </c>
-      <c r="M11" s="1">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="5"/>
+      <c r="M11" s="10">
+        <v>1</v>
+      </c>
+      <c r="N11" s="10">
+        <v>1</v>
+      </c>
+      <c r="O11" s="6">
+        <f t="shared" si="10"/>
         <v>0.99999999999999978</v>
       </c>
-      <c r="P11">
-        <f t="shared" si="6"/>
+      <c r="P11" s="6">
+        <f t="shared" si="11"/>
         <v>0.27999999999999997</v>
       </c>
-      <c r="Q11" s="3">
-        <f>K11-1+(M11/(3*10^5))</f>
+      <c r="Q11" s="9">
+        <f t="shared" si="12"/>
         <v>3.3333333333333333e-06</v>
       </c>
-      <c r="R11">
-        <f>C11+(Q11*I11)</f>
+      <c r="R11" s="6">
+        <f t="shared" si="13"/>
         <v>1.8100009333333333</v>
       </c>
-      <c r="S11">
-        <f>R11+(O11*I11)</f>
+      <c r="S11" s="6">
+        <f t="shared" si="14"/>
         <v>2.0900009333333331</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="T11" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" ht="14.25">
+    <row r="12" s="6" customFormat="1" ht="14.25">
       <c r="A12" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>1.47</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>4.3639999999999999</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <v>3.9870000000000001</v>
       </c>
-      <c r="F12" s="4">
-        <f t="shared" si="3"/>
+      <c r="F12" s="8">
+        <f t="shared" si="7"/>
         <v>0.37699999999999978</v>
       </c>
-      <c r="G12" s="3">
-        <f t="shared" si="4"/>
+      <c r="G12" s="9">
+        <f t="shared" si="8"/>
         <v>25.646258503401349</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="6">
         <v>3</v>
       </c>
-      <c r="I12">
-        <f>F12/H12</f>
+      <c r="I12" s="6">
+        <f t="shared" si="9"/>
         <v>0.12566666666666659</v>
       </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
+      <c r="J12" s="6">
+        <v>1</v>
+      </c>
+      <c r="K12" s="6">
+        <v>1</v>
+      </c>
+      <c r="L12" s="6">
         <v>3</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="10">
         <f>1*10^5</f>
         <v>100000</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="10">
         <f>1.5*10^5</f>
         <v>150000</v>
       </c>
-      <c r="O12">
-        <f>(L12+((N12+(5*10^4))/(3*10^5))-(K12+((M12+(5*10^4))/(3*10^5))))</f>
+      <c r="O12" s="6">
+        <f t="shared" si="10"/>
         <v>2.1666666666666665</v>
       </c>
-      <c r="P12">
-        <f>O12*I12</f>
+      <c r="P12" s="6">
+        <f t="shared" si="11"/>
         <v>0.27227777777777762</v>
       </c>
-      <c r="Q12" s="3">
-        <f>K12-1+(M12/(3*10^5))</f>
+      <c r="Q12" s="9">
+        <f t="shared" si="12"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="R12">
-        <f>C12+(Q12*I12)</f>
+      <c r="R12" s="6">
+        <f t="shared" si="13"/>
         <v>1.5118888888888888</v>
       </c>
-      <c r="S12">
-        <f>R12+(O12*I12)</f>
+      <c r="S12" s="6">
+        <f t="shared" si="14"/>
         <v>1.7841666666666665</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" ht="14.25">
+      <c r="A13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>1.79</v>
+      </c>
+      <c r="D13">
+        <v>4.6079999999999997</v>
+      </c>
+      <c r="E13">
+        <v>3.653</v>
+      </c>
       <c r="F13" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="3" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I13" t="e">
-        <f>F13/H13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S13" t="e">
-        <f>R13+(O13*I13)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="7"/>
+        <v>0.95499999999999963</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="8"/>
+        <v>53.351955307262543</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="9"/>
+        <v>0.23874999999999991</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="9">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="R13" s="6">
+        <f t="shared" si="13"/>
+        <v>1.55125</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="14"/>
+        <v>1.55125</v>
+      </c>
+      <c r="T13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" ht="14.25">
+      <c r="A14" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>2.71</v>
+      </c>
+      <c r="D14">
+        <v>4.7290000000000001</v>
+      </c>
+      <c r="E14">
+        <v>4.5599999999999996</v>
+      </c>
       <c r="F14" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="3" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I14" t="e">
-        <f>F14/H14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S14" t="e">
-        <f>R14+(O14*I14)</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="7"/>
+        <v>0.16900000000000048</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="8"/>
+        <v>6.2361623616236344</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="9"/>
+        <v>0.056333333333333492</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="M14" s="5">
+        <f>1*10^5</f>
+        <v>100000</v>
+      </c>
+      <c r="N14" s="5">
+        <f>2.5*10^4</f>
+        <v>25000</v>
+      </c>
+      <c r="O14" s="6">
+        <f t="shared" si="10"/>
+        <v>1.75</v>
+      </c>
+      <c r="P14" s="6">
+        <f t="shared" si="11"/>
+        <v>0.098583333333333606</v>
+      </c>
+      <c r="Q14" s="9">
+        <f t="shared" si="12"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="R14" s="6">
+        <f t="shared" si="13"/>
+        <v>2.7287777777777777</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="14"/>
+        <v>2.8273611111111112</v>
+      </c>
+      <c r="T14" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="F15" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G15" s="3" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I15" t="e">
-        <f>F15/H15</f>
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q15" s="9">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="R15" s="6" t="e">
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S15" t="e">
-        <f>R15+(O15*I15)</f>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="F16" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G16" s="3" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I16" t="e">
-        <f>F16/H16</f>
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q16" s="9">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="R16" s="6" t="e">
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S16" t="e">
-        <f>R16+(O16*I16)</f>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" ht="14.25">
       <c r="F17" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G17" s="3" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I17" t="e">
-        <f>F17/H17</f>
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q17" s="9">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="R17" s="6" t="e">
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S17" t="e">
-        <f>R17+(O17*I17)</f>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="F18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G18" s="3" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I18" t="e">
-        <f>F18/H18</f>
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q18" s="9">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="R18" s="6" t="e">
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S18" t="e">
-        <f>R18+(O18*I18)</f>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="F19" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G19" s="3" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I19" t="e">
-        <f>F19/H19</f>
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M19" s="5"/>
+      <c r="O19" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q19" s="9">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="R19" s="6" t="e">
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S19" t="e">
-        <f>R19+(O19*I19)</f>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="S20">
-        <f>R20+(O20*I20)</f>
-        <v>0</v>
+      <c r="F20" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="3" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O20" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q20" s="9">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="R20" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S20" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="S21">
-        <f>R21+(O21*I21)</f>
-        <v>0</v>
+      <c r="F21" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="3" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O21" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P21" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q21" s="9">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="R21" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S21" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="S22">
-        <f>R22+(O22*I22)</f>
-        <v>0</v>
+      <c r="F22" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="3" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O22" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q22" s="9">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="R22" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S22" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="S23">
-        <f>R23+(O23*I23)</f>
-        <v>0</v>
+      <c r="F23" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="3" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O23" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q23" s="9">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="R23" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S23" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" ht="14.25">
+      <c r="F24" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="3" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I24" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="J24" s="1"/>
-      <c r="S24">
-        <f>R24+(O24*I24)</f>
-        <v>0</v>
+      <c r="O24" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q24" s="9">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="R24" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S24" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="D25" s="1"/>
+      <c r="F25" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="3" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O25" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P25" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q25" s="9">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="R25" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S25" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="D26" s="1"/>
+      <c r="F26" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="3" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I26" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O26" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P26" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q26" s="9">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="R26" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S26" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27">
+        <v>2.6800000000000002</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4.1699999999999999</v>
+      </c>
+      <c r="E27">
+        <v>3.8199999999999998</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="7"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="G27" s="3">
+        <f t="shared" si="8"/>
+        <v>13.059701492537314</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="9"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <f>1*10^5</f>
+        <v>100000</v>
+      </c>
+      <c r="N27">
+        <f>3.75*10^5</f>
+        <v>375000</v>
+      </c>
+      <c r="O27" s="6">
+        <f t="shared" ref="O27:O30" si="15">(L27+((N27+(5*10^4))/(6*10^5))-(K27+((M27+(5*10^4))/(6*10^5))))</f>
+        <v>0.45833333333333348</v>
+      </c>
+      <c r="P27" s="6">
+        <f t="shared" si="11"/>
+        <v>0.16041666666666676</v>
+      </c>
+      <c r="Q27" s="9">
+        <f t="shared" si="12"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="R27" s="6">
+        <f t="shared" si="13"/>
+        <v>2.7966666666666669</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="14"/>
+        <v>2.9570833333333337</v>
+      </c>
+      <c r="T27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28">
+        <v>1.25</v>
+      </c>
+      <c r="D28">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="E28">
+        <v>3.8599999999999999</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="7"/>
+        <v>0.48999999999999977</v>
+      </c>
+      <c r="G28" s="3">
+        <f t="shared" si="8"/>
+        <v>39.199999999999982</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="9"/>
+        <v>0.48999999999999977</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <f>5*10^5</f>
+        <v>500000</v>
+      </c>
+      <c r="O28" s="6">
+        <f t="shared" si="15"/>
+        <v>0.83333166666666658</v>
+      </c>
+      <c r="P28" s="6">
+        <f t="shared" si="11"/>
+        <v>0.40833251666666642</v>
+      </c>
+      <c r="Q28" s="9">
+        <f t="shared" si="12"/>
+        <v>3.3333333333333333e-06</v>
+      </c>
+      <c r="R28" s="6">
+        <f t="shared" si="13"/>
+        <v>1.2500016333333333</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="14"/>
+        <v>1.6583341499999997</v>
+      </c>
+      <c r="T28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29">
+        <v>2.0899999999999999</v>
+      </c>
+      <c r="D29">
+        <v>3.96</v>
+      </c>
+      <c r="E29">
+        <v>3.4500000000000002</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" si="7"/>
+        <v>0.50999999999999979</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" si="8"/>
+        <v>24.401913875598076</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="9"/>
+        <v>0.50999999999999979</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <f>4*10^5</f>
+        <v>400000</v>
+      </c>
+      <c r="O29" s="6">
+        <f t="shared" si="15"/>
+        <v>0.66666500000000006</v>
+      </c>
+      <c r="P29" s="6">
+        <f t="shared" si="11"/>
+        <v>0.33999914999999992</v>
+      </c>
+      <c r="Q29" s="9">
+        <f t="shared" si="12"/>
+        <v>3.3333333333333333e-06</v>
+      </c>
+      <c r="R29" s="6">
+        <f t="shared" si="13"/>
+        <v>2.0900016999999997</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="14"/>
+        <v>2.4300008499999999</v>
+      </c>
+      <c r="T29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="A30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30">
+        <v>3.02</v>
+      </c>
+      <c r="D30">
+        <v>4.4299999999999997</v>
+      </c>
+      <c r="E30">
+        <v>3.9199999999999999</v>
+      </c>
+      <c r="F30" s="4">
+        <f t="shared" si="7"/>
+        <v>0.50999999999999979</v>
+      </c>
+      <c r="G30" s="3">
+        <f t="shared" si="8"/>
+        <v>16.887417218543039</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="9"/>
+        <v>0.50999999999999979</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <f>4.6*10^5</f>
+        <v>459999.99999999994</v>
+      </c>
+      <c r="O30" s="6">
+        <f t="shared" si="15"/>
+        <v>0.76666499999999993</v>
+      </c>
+      <c r="P30" s="6">
+        <f t="shared" si="11"/>
+        <v>0.3909991499999998</v>
+      </c>
+      <c r="Q30" s="9">
+        <f t="shared" si="12"/>
+        <v>3.3333333333333333e-06</v>
+      </c>
+      <c r="R30" s="6">
+        <f t="shared" si="13"/>
+        <v>3.0200016999999999</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="14"/>
+        <v>3.4110008499999998</v>
+      </c>
+      <c r="T30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="F31" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="3" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="F32" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="3" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I32" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing some analytical bugs
</commit_message>
<xml_diff>
--- a/FatMothSet1Guide.xlsx
+++ b/FatMothSet1Guide.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -154,10 +154,16 @@
     <t xml:space="preserve">meh behavior</t>
   </si>
   <si>
+    <t>2024_12_04_1</t>
+  </si>
+  <si>
+    <t>2024_12_04_2</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
     <t>2024_08_01</t>
-  </si>
-  <si>
-    <t>Female</t>
   </si>
   <si>
     <t>COLD!</t>
@@ -194,7 +200,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +211,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.14999847407452621"/>
+        <bgColor theme="2" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
   </fills>
@@ -227,7 +239,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -264,7 +276,16 @@
     <xf fontId="0" fillId="2" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
@@ -701,7 +722,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" topLeftCell="G1" zoomScale="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" topLeftCell="A5" zoomScale="100" workbookViewId="0">
       <selection activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -1477,90 +1498,111 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" ht="14.25">
+    <row r="14" s="12" customFormat="1" ht="14.25">
       <c r="A14" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="12">
         <v>2.71</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="12">
         <v>4.7290000000000001</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="12">
         <v>4.5599999999999996</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="13">
         <f t="shared" si="7"/>
         <v>0.16900000000000048</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="14">
         <f t="shared" si="8"/>
         <v>6.2361623616236344</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="12">
         <v>3</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="12">
         <f t="shared" si="9"/>
         <v>0.056333333333333492</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
+      <c r="J14" s="12">
+        <v>1</v>
+      </c>
+      <c r="K14" s="12">
+        <v>1</v>
+      </c>
+      <c r="L14" s="12">
         <v>3</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="15">
         <f>1*10^5</f>
         <v>100000</v>
       </c>
-      <c r="N14" s="5">
-        <f>2.5*10^4</f>
-        <v>25000</v>
-      </c>
-      <c r="O14" s="6">
+      <c r="N14" s="15">
+        <f>1.5*10^5</f>
+        <v>150000</v>
+      </c>
+      <c r="O14" s="12">
         <f t="shared" si="10"/>
-        <v>1.75</v>
-      </c>
-      <c r="P14" s="6">
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="P14" s="12">
         <f t="shared" si="11"/>
-        <v>0.098583333333333606</v>
-      </c>
-      <c r="Q14" s="9">
+        <v>0.12205555555555589</v>
+      </c>
+      <c r="Q14" s="14">
         <f t="shared" si="12"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="R14" s="6">
+      <c r="R14" s="12">
         <f t="shared" si="13"/>
         <v>2.7287777777777777</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="12">
         <f t="shared" si="14"/>
-        <v>2.8273611111111112</v>
-      </c>
-      <c r="T14" t="s">
+        <v>2.8508333333333336</v>
+      </c>
+      <c r="T14" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" ht="14.25">
+      <c r="A15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>2.6099999999999999</v>
+      </c>
+      <c r="D15">
+        <v>4.6920000000000002</v>
+      </c>
+      <c r="E15">
+        <v>4.2720000000000002</v>
+      </c>
       <c r="F15" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="3" t="e">
+        <v>0.41999999999999993</v>
+      </c>
+      <c r="G15" s="3">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I15" t="e">
+        <v>16.091954022988503</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
@@ -1568,57 +1610,89 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P15" s="6" t="e">
+      <c r="P15" s="6">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="9">
         <f t="shared" si="12"/>
         <v>-1</v>
       </c>
-      <c r="R15" s="6" t="e">
+      <c r="R15" s="6">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S15" t="e">
+        <v>2.4699999999999998</v>
+      </c>
+      <c r="S15">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25">
-      <c r="F16" s="4">
+        <v>2.4699999999999998</v>
+      </c>
+    </row>
+    <row r="16" s="12" customFormat="1" ht="14.25">
+      <c r="A16" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="12">
+        <v>2.79</v>
+      </c>
+      <c r="D16" s="12">
+        <v>4.2590000000000003</v>
+      </c>
+      <c r="E16" s="12">
+        <v>3.4750000000000001</v>
+      </c>
+      <c r="F16" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="3" t="e">
+        <v>0.78400000000000025</v>
+      </c>
+      <c r="G16" s="14">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I16" t="e">
+        <v>28.100358422939074</v>
+      </c>
+      <c r="H16" s="12">
+        <v>4</v>
+      </c>
+      <c r="I16" s="12">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="6">
+        <v>0.19600000000000006</v>
+      </c>
+      <c r="J16" s="12">
+        <v>1</v>
+      </c>
+      <c r="K16" s="12">
+        <v>1</v>
+      </c>
+      <c r="L16" s="12">
+        <v>4</v>
+      </c>
+      <c r="M16" s="15">
+        <v>1</v>
+      </c>
+      <c r="N16" s="15">
+        <f>1.2*10^5</f>
+        <v>120000</v>
+      </c>
+      <c r="O16" s="12">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="6" t="e">
+        <v>3.3999966666666666</v>
+      </c>
+      <c r="P16" s="12">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q16" s="9">
+        <v>0.66639934666666689</v>
+      </c>
+      <c r="Q16" s="14">
         <f t="shared" si="12"/>
-        <v>-1</v>
-      </c>
-      <c r="R16" s="6" t="e">
+        <v>3.3333333333333333e-06</v>
+      </c>
+      <c r="R16" s="12">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S16" t="e">
+        <v>2.7900006533333332</v>
+      </c>
+      <c r="S16" s="12">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>3.4564000000000004</v>
       </c>
     </row>
     <row r="17" ht="14.25">
@@ -1971,10 +2045,10 @@
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C27">
         <v>2.6800000000000002</v>
@@ -2038,12 +2112,12 @@
         <v>2.9570833333333337</v>
       </c>
       <c r="T27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>19</v>
@@ -2109,15 +2183,15 @@
         <v>1.6583341499999997</v>
       </c>
       <c r="T28" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C29">
         <v>2.0899999999999999</v>
@@ -2180,15 +2254,15 @@
         <v>2.4300008499999999</v>
       </c>
       <c r="T29" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C30">
         <v>3.02</v>
@@ -2251,7 +2325,7 @@
         <v>3.4110008499999998</v>
       </c>
       <c r="T30" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" ht="14.25">
@@ -2280,6 +2354,37 @@
       <c r="I32" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="E35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="E36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="E37">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38"/>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="E39">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="E40">
+        <v>1101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pre Sicb Figure Making
</commit_message>
<xml_diff>
--- a/FatMothSet1Guide.xlsx
+++ b/FatMothSet1Guide.xlsx
@@ -189,7 +189,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -199,8 +199,12 @@
       <sz val="10.000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11.000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +221,12 @@
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.14999847407452621"/>
         <bgColor theme="2" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="0"/>
+        <bgColor theme="0" tint="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -239,7 +249,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -276,6 +286,9 @@
     <xf fontId="0" fillId="2" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -286,6 +299,18 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="2" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="2" fillId="4" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="2" fillId="4" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="2" fillId="4" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
@@ -722,7 +747,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" topLeftCell="A5" zoomScale="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" zoomScale="100" workbookViewId="0">
       <selection activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -1227,7 +1252,7 @@
       </c>
     </row>
     <row r="10" s="6" customFormat="1" ht="14.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -1343,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="O11" s="6">
-        <f t="shared" si="10"/>
+        <f>(L11+((N11+(5*10^4))/(3*10^5))-(K11+((M11+(5*10^4))/(3*10^5))))</f>
         <v>0.99999999999999978</v>
       </c>
       <c r="P11" s="6">
@@ -1498,75 +1523,75 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" s="12" customFormat="1" ht="14.25">
-      <c r="A14" s="12" t="s">
+    <row r="14" s="13" customFormat="1" ht="14.25">
+      <c r="A14" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="13">
         <v>2.71</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="13">
         <v>4.7290000000000001</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="13">
         <v>4.5599999999999996</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="14">
         <f t="shared" si="7"/>
         <v>0.16900000000000048</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="15">
         <f t="shared" si="8"/>
         <v>6.2361623616236344</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="13">
         <v>3</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="13">
         <f t="shared" si="9"/>
         <v>0.056333333333333492</v>
       </c>
-      <c r="J14" s="12">
-        <v>1</v>
-      </c>
-      <c r="K14" s="12">
-        <v>1</v>
-      </c>
-      <c r="L14" s="12">
+      <c r="J14" s="13">
+        <v>1</v>
+      </c>
+      <c r="K14" s="13">
+        <v>1</v>
+      </c>
+      <c r="L14" s="13">
         <v>3</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M14" s="16">
         <f>1*10^5</f>
         <v>100000</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="16">
         <f>1.5*10^5</f>
         <v>150000</v>
       </c>
-      <c r="O14" s="12">
+      <c r="O14" s="13">
         <f t="shared" si="10"/>
         <v>2.1666666666666665</v>
       </c>
-      <c r="P14" s="12">
+      <c r="P14" s="13">
         <f t="shared" si="11"/>
         <v>0.12205555555555589</v>
       </c>
-      <c r="Q14" s="14">
+      <c r="Q14" s="15">
         <f t="shared" si="12"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="R14" s="12">
+      <c r="R14" s="13">
         <f t="shared" si="13"/>
         <v>2.7287777777777777</v>
       </c>
-      <c r="S14" s="12">
+      <c r="S14" s="13">
         <f t="shared" si="14"/>
         <v>2.8508333333333336</v>
       </c>
-      <c r="T14" s="12" t="s">
+      <c r="T14" s="13" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1627,70 +1652,70 @@
         <v>2.4699999999999998</v>
       </c>
     </row>
-    <row r="16" s="12" customFormat="1" ht="14.25">
-      <c r="A16" s="12" t="s">
+    <row r="16" s="17" customFormat="1" ht="14.25">
+      <c r="A16" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="17">
         <v>2.79</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="17">
         <v>4.2590000000000003</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="17">
         <v>3.4750000000000001</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="18">
         <f t="shared" si="7"/>
         <v>0.78400000000000025</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="19">
         <f t="shared" si="8"/>
         <v>28.100358422939074</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="17">
         <v>4</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="17">
         <f t="shared" si="9"/>
         <v>0.19600000000000006</v>
       </c>
-      <c r="J16" s="12">
-        <v>1</v>
-      </c>
-      <c r="K16" s="12">
-        <v>1</v>
-      </c>
-      <c r="L16" s="12">
+      <c r="J16" s="17">
+        <v>1</v>
+      </c>
+      <c r="K16" s="17">
+        <v>1</v>
+      </c>
+      <c r="L16" s="17">
         <v>4</v>
       </c>
-      <c r="M16" s="15">
-        <v>1</v>
-      </c>
-      <c r="N16" s="15">
+      <c r="M16" s="20">
+        <v>1</v>
+      </c>
+      <c r="N16" s="20">
         <f>1.2*10^5</f>
         <v>120000</v>
       </c>
-      <c r="O16" s="12">
+      <c r="O16" s="17">
         <f t="shared" si="10"/>
         <v>3.3999966666666666</v>
       </c>
-      <c r="P16" s="12">
+      <c r="P16" s="17">
         <f t="shared" si="11"/>
         <v>0.66639934666666689</v>
       </c>
-      <c r="Q16" s="14">
+      <c r="Q16" s="19">
         <f t="shared" si="12"/>
         <v>3.3333333333333333e-06</v>
       </c>
-      <c r="R16" s="12">
+      <c r="R16" s="17">
         <f t="shared" si="13"/>
         <v>2.7900006533333332</v>
       </c>
-      <c r="S16" s="12">
+      <c r="S16" s="17">
         <f t="shared" si="14"/>
         <v>3.4564000000000004</v>
       </c>
@@ -2356,37 +2381,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" ht="14.25">
-      <c r="E35">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" ht="14.25">
-      <c r="E36">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" ht="14.25">
-      <c r="E37">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" ht="14.25">
-      <c r="E38">
-        <v>5</v>
-      </c>
-      <c r="F38"/>
-    </row>
-    <row r="39" ht="14.25">
-      <c r="E39">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="40" ht="14.25">
-      <c r="E40">
-        <v>1101</v>
-      </c>
-    </row>
+    <row r="35" ht="14.25"/>
+    <row r="36" ht="14.25"/>
+    <row r="37" ht="14.25"/>
+    <row r="38" ht="14.25"/>
+    <row r="39" ht="14.25"/>
+    <row r="40" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins left="0.70069444444444484" right="0.70069444444444484" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51181102362204689" footer="0.51181102362204689"/>

</xml_diff>

<commit_message>
Fixed PCA Pipeline by more heavily relying on Leo's Code, Moved Good Tracking Params from manual extraction from .xlsx to a dict in the new_single_moth pipeline
</commit_message>
<xml_diff>
--- a/FatMothSet1Guide.xlsx
+++ b/FatMothSet1Guide.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -163,6 +163,12 @@
     <t>Female</t>
   </si>
   <si>
+    <t>2025_01_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great Behavior Clean Muscles Just Dropped Z Force SMH </t>
+  </si>
+  <si>
     <t>2024_08_01</t>
   </si>
   <si>
@@ -179,6 +185,12 @@
   </si>
   <si>
     <t>2024_06_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check 1104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check 1120 </t>
   </si>
 </sst>
 </file>
@@ -286,9 +298,6 @@
     <xf fontId="0" fillId="2" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -311,6 +320,9 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="2" fillId="4" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
@@ -1252,7 +1264,7 @@
       </c>
     </row>
     <row r="10" s="6" customFormat="1" ht="14.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -1368,7 +1380,7 @@
         <v>1</v>
       </c>
       <c r="O11" s="6">
-        <f>(L11+((N11+(5*10^4))/(3*10^5))-(K11+((M11+(5*10^4))/(3*10^5))))</f>
+        <f t="shared" si="10"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="P11" s="6">
@@ -1523,75 +1535,75 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" s="13" customFormat="1" ht="14.25">
-      <c r="A14" s="13" t="s">
+    <row r="14" s="12" customFormat="1" ht="14.25">
+      <c r="A14" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="12">
         <v>2.71</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="12">
         <v>4.7290000000000001</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <v>4.5599999999999996</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="13">
         <f t="shared" si="7"/>
         <v>0.16900000000000048</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="14">
         <f t="shared" si="8"/>
         <v>6.2361623616236344</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="12">
         <v>3</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="12">
         <f t="shared" si="9"/>
         <v>0.056333333333333492</v>
       </c>
-      <c r="J14" s="13">
-        <v>1</v>
-      </c>
-      <c r="K14" s="13">
-        <v>1</v>
-      </c>
-      <c r="L14" s="13">
+      <c r="J14" s="12">
+        <v>1</v>
+      </c>
+      <c r="K14" s="12">
+        <v>1</v>
+      </c>
+      <c r="L14" s="12">
         <v>3</v>
       </c>
-      <c r="M14" s="16">
+      <c r="M14" s="15">
         <f>1*10^5</f>
         <v>100000</v>
       </c>
-      <c r="N14" s="16">
+      <c r="N14" s="15">
         <f>1.5*10^5</f>
         <v>150000</v>
       </c>
-      <c r="O14" s="13">
+      <c r="O14" s="12">
         <f t="shared" si="10"/>
         <v>2.1666666666666665</v>
       </c>
-      <c r="P14" s="13">
+      <c r="P14" s="12">
         <f t="shared" si="11"/>
         <v>0.12205555555555589</v>
       </c>
-      <c r="Q14" s="15">
+      <c r="Q14" s="14">
         <f t="shared" si="12"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="R14" s="13">
+      <c r="R14" s="12">
         <f t="shared" si="13"/>
         <v>2.7287777777777777</v>
       </c>
-      <c r="S14" s="13">
+      <c r="S14" s="12">
         <f t="shared" si="14"/>
         <v>2.8508333333333336</v>
       </c>
-      <c r="T14" s="13" t="s">
+      <c r="T14" s="12" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1652,108 +1664,142 @@
         <v>2.4699999999999998</v>
       </c>
     </row>
-    <row r="16" s="17" customFormat="1" ht="14.25">
-      <c r="A16" s="17" t="s">
+    <row r="16" s="16" customFormat="1" ht="14.25">
+      <c r="A16" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="16">
         <v>2.79</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <v>4.2590000000000003</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="16">
         <v>3.4750000000000001</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="17">
         <f t="shared" si="7"/>
         <v>0.78400000000000025</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="18">
         <f t="shared" si="8"/>
         <v>28.100358422939074</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="16">
         <v>4</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="16">
         <f t="shared" si="9"/>
         <v>0.19600000000000006</v>
       </c>
-      <c r="J16" s="17">
-        <v>1</v>
-      </c>
-      <c r="K16" s="17">
-        <v>1</v>
-      </c>
-      <c r="L16" s="17">
+      <c r="J16" s="16">
+        <v>1</v>
+      </c>
+      <c r="K16" s="16">
+        <v>1</v>
+      </c>
+      <c r="L16" s="16">
         <v>4</v>
       </c>
-      <c r="M16" s="20">
-        <v>1</v>
-      </c>
-      <c r="N16" s="20">
+      <c r="M16" s="19">
+        <v>1</v>
+      </c>
+      <c r="N16" s="19">
         <f>1.2*10^5</f>
         <v>120000</v>
       </c>
-      <c r="O16" s="17">
+      <c r="O16" s="16">
         <f t="shared" si="10"/>
         <v>3.3999966666666666</v>
       </c>
-      <c r="P16" s="17">
+      <c r="P16" s="16">
         <f t="shared" si="11"/>
         <v>0.66639934666666689</v>
       </c>
-      <c r="Q16" s="19">
+      <c r="Q16" s="18">
         <f t="shared" si="12"/>
         <v>3.3333333333333333e-06</v>
       </c>
-      <c r="R16" s="17">
+      <c r="R16" s="16">
         <f t="shared" si="13"/>
         <v>2.7900006533333332</v>
       </c>
-      <c r="S16" s="17">
+      <c r="S16" s="16">
         <f t="shared" si="14"/>
         <v>3.4564000000000004</v>
       </c>
     </row>
     <row r="17" ht="14.25">
-      <c r="F17" s="4">
+      <c r="A17" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="12">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="D17" s="12">
+        <v>4.6429999999999998</v>
+      </c>
+      <c r="E17" s="12">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="F17" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="3" t="e">
+        <v>0.50300000000000011</v>
+      </c>
+      <c r="G17" s="14">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I17" t="e">
+        <v>24.299516908212567</v>
+      </c>
+      <c r="H17" s="12">
+        <v>2</v>
+      </c>
+      <c r="I17" s="12">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="6">
+        <v>0.25150000000000006</v>
+      </c>
+      <c r="J17" s="12">
+        <v>1</v>
+      </c>
+      <c r="K17" s="12">
+        <v>1</v>
+      </c>
+      <c r="L17" s="12">
+        <v>2</v>
+      </c>
+      <c r="M17" s="15">
+        <v>1</v>
+      </c>
+      <c r="N17" s="15">
+        <v>150000</v>
+      </c>
+      <c r="O17" s="12">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="6" t="e">
+        <v>1.4999966666666664</v>
+      </c>
+      <c r="P17" s="12">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q17" s="9">
+        <v>0.37724916166666667</v>
+      </c>
+      <c r="Q17" s="14">
         <f t="shared" si="12"/>
-        <v>-1</v>
-      </c>
-      <c r="R17" s="6" t="e">
+        <v>3.3333333333333333e-06</v>
+      </c>
+      <c r="R17" s="12">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S17" t="e">
+        <v>2.0700008383333333</v>
+      </c>
+      <c r="S17" s="12">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>2.4472499999999999</v>
+      </c>
+      <c r="T17" s="12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18" ht="14.25">
@@ -2070,7 +2116,7 @@
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>47</v>
@@ -2137,12 +2183,12 @@
         <v>2.9570833333333337</v>
       </c>
       <c r="T27" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>19</v>
@@ -2208,12 +2254,12 @@
         <v>1.6583341499999997</v>
       </c>
       <c r="T28" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>47</v>
@@ -2279,12 +2325,12 @@
         <v>2.4300008499999999</v>
       </c>
       <c r="T29" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>47</v>
@@ -2350,7 +2396,7 @@
         <v>3.4110008499999998</v>
       </c>
       <c r="T30" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" ht="14.25">
@@ -2381,12 +2427,22 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" ht="14.25"/>
+    <row r="34" ht="14.25">
+      <c r="I34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="I35" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="36" ht="14.25"/>
     <row r="37" ht="14.25"/>
     <row r="38" ht="14.25"/>
     <row r="39" ht="14.25"/>
     <row r="40" ht="14.25"/>
+    <row r="45" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins left="0.70069444444444484" right="0.70069444444444484" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51181102362204689" footer="0.51181102362204689"/>

</xml_diff>

<commit_message>
Cleaned up Single Moth analysis, coord pattern findings
</commit_message>
<xml_diff>
--- a/FatMothSet1Guide.xlsx
+++ b/FatMothSet1Guide.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t xml:space="preserve">Great Behavior Clean Muscles Just Dropped Z Force SMH </t>
+  </si>
+  <si>
+    <t>2025_01_30</t>
   </si>
   <si>
     <t>2024_08_01</t>
@@ -231,14 +234,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.14999847407452621"/>
-        <bgColor theme="2" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="0"/>
+        <bgColor theme="0" tint="0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="0"/>
-        <bgColor theme="0" tint="0"/>
+        <fgColor theme="2" tint="-0.14999847407452621"/>
+        <bgColor theme="2" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
   </fills>
@@ -261,7 +264,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -310,19 +313,31 @@
     <xf fontId="0" fillId="3" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="2" fillId="4" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="2" fillId="4" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="2" fillId="4" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="0">
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
@@ -1739,103 +1754,134 @@
       <c r="B17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="20">
         <v>2.0699999999999998</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="20">
         <v>4.6429999999999998</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="20">
         <v>4.1399999999999997</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="21">
         <f t="shared" si="7"/>
         <v>0.50300000000000011</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="22">
         <f t="shared" si="8"/>
         <v>24.299516908212567</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="20">
         <v>2</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="20">
         <f t="shared" si="9"/>
         <v>0.25150000000000006</v>
       </c>
-      <c r="J17" s="12">
-        <v>1</v>
-      </c>
-      <c r="K17" s="12">
-        <v>1</v>
-      </c>
-      <c r="L17" s="12">
+      <c r="J17" s="20">
+        <v>1</v>
+      </c>
+      <c r="K17" s="20">
+        <v>1</v>
+      </c>
+      <c r="L17" s="20">
         <v>2</v>
       </c>
-      <c r="M17" s="15">
-        <v>1</v>
-      </c>
-      <c r="N17" s="15">
+      <c r="M17" s="23">
+        <v>1</v>
+      </c>
+      <c r="N17" s="23">
         <v>150000</v>
       </c>
-      <c r="O17" s="12">
+      <c r="O17" s="20">
         <f t="shared" si="10"/>
         <v>1.4999966666666664</v>
       </c>
-      <c r="P17" s="12">
+      <c r="P17" s="20">
         <f t="shared" si="11"/>
         <v>0.37724916166666667</v>
       </c>
-      <c r="Q17" s="14">
+      <c r="Q17" s="22">
         <f t="shared" si="12"/>
         <v>3.3333333333333333e-06</v>
       </c>
-      <c r="R17" s="12">
+      <c r="R17" s="20">
         <f t="shared" si="13"/>
         <v>2.0700008383333333</v>
       </c>
-      <c r="S17" s="12">
+      <c r="S17" s="20">
         <f t="shared" si="14"/>
         <v>2.4472499999999999</v>
       </c>
-      <c r="T17" s="12" t="s">
+      <c r="T17" s="20" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="18" ht="14.25">
+      <c r="A18" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>2.1200000000000001</v>
+      </c>
+      <c r="D18">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="E18">
+        <v>3.8380000000000001</v>
+      </c>
       <c r="F18" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="3" t="e">
+        <v>0.60200000000000031</v>
+      </c>
+      <c r="G18" s="3">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" t="e">
+        <v>28.396226415094354</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
+        <v>0.30100000000000016</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18" s="5">
+        <v>10000</v>
+      </c>
+      <c r="N18" s="5">
+        <v>125000</v>
+      </c>
       <c r="O18" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P18" s="6" t="e">
+        <v>1.3833333333333335</v>
+      </c>
+      <c r="P18" s="6">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0.41638333333333361</v>
       </c>
       <c r="Q18" s="9">
         <f t="shared" si="12"/>
-        <v>-1</v>
-      </c>
-      <c r="R18" s="6" t="e">
+        <v>0.033333333333333333</v>
+      </c>
+      <c r="R18" s="6">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S18" t="e">
+        <v>2.1300333333333334</v>
+      </c>
+      <c r="S18">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>2.546416666666667</v>
       </c>
     </row>
     <row r="19" ht="14.25">
@@ -2116,7 +2162,7 @@
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>47</v>
@@ -2183,12 +2229,12 @@
         <v>2.9570833333333337</v>
       </c>
       <c r="T27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>19</v>
@@ -2254,12 +2300,12 @@
         <v>1.6583341499999997</v>
       </c>
       <c r="T28" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>47</v>
@@ -2325,12 +2371,12 @@
         <v>2.4300008499999999</v>
       </c>
       <c r="T29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>47</v>
@@ -2396,7 +2442,7 @@
         <v>3.4110008499999998</v>
       </c>
       <c r="T30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" ht="14.25">
@@ -2429,12 +2475,12 @@
     </row>
     <row r="34" ht="14.25">
       <c r="I34" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" ht="14.25">
       <c r="I35" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" ht="14.25"/>

</xml_diff>

<commit_message>
Complete Overhaul and Restructure and Cleaning it out
</commit_message>
<xml_diff>
--- a/FatMothSet1Guide.xlsx
+++ b/FatMothSet1Guide.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t>2025_01_30</t>
+  </si>
+  <si>
+    <t>2025_03_20</t>
+  </si>
+  <si>
+    <t>2025_04_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male </t>
   </si>
   <si>
     <t>2024_08_01</t>
@@ -219,7 +228,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,12 +245,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="0"/>
         <bgColor theme="0" tint="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.14999847407452621"/>
-        <bgColor theme="2" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
   </fills>
@@ -264,7 +267,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="20">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -323,21 +326,6 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
@@ -1747,81 +1735,81 @@
         <v>3.4564000000000004</v>
       </c>
     </row>
-    <row r="17" ht="14.25">
-      <c r="A17" s="20" t="s">
+    <row r="17" s="6" customFormat="1" ht="14.25">
+      <c r="A17" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="6">
         <v>2.0699999999999998</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="6">
         <v>4.6429999999999998</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="6">
         <v>4.1399999999999997</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="8">
         <f t="shared" si="7"/>
         <v>0.50300000000000011</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="9">
         <f t="shared" si="8"/>
         <v>24.299516908212567</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="6">
         <v>2</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I17" s="6">
         <f t="shared" si="9"/>
         <v>0.25150000000000006</v>
       </c>
-      <c r="J17" s="20">
-        <v>1</v>
-      </c>
-      <c r="K17" s="20">
-        <v>1</v>
-      </c>
-      <c r="L17" s="20">
+      <c r="J17" s="6">
+        <v>1</v>
+      </c>
+      <c r="K17" s="6">
+        <v>1</v>
+      </c>
+      <c r="L17" s="6">
         <v>2</v>
       </c>
-      <c r="M17" s="23">
-        <v>1</v>
-      </c>
-      <c r="N17" s="23">
-        <v>150000</v>
-      </c>
-      <c r="O17" s="20">
+      <c r="M17" s="10">
+        <v>1</v>
+      </c>
+      <c r="N17" s="10">
+        <v>250000</v>
+      </c>
+      <c r="O17" s="6">
         <f t="shared" si="10"/>
-        <v>1.4999966666666664</v>
-      </c>
-      <c r="P17" s="20">
+        <v>1.8333299999999999</v>
+      </c>
+      <c r="P17" s="6">
         <f t="shared" si="11"/>
-        <v>0.37724916166666667</v>
-      </c>
-      <c r="Q17" s="22">
+        <v>0.46108249500000009</v>
+      </c>
+      <c r="Q17" s="9">
         <f t="shared" si="12"/>
         <v>3.3333333333333333e-06</v>
       </c>
-      <c r="R17" s="20">
+      <c r="R17" s="6">
         <f t="shared" si="13"/>
         <v>2.0700008383333333</v>
       </c>
-      <c r="S17" s="20">
+      <c r="S17" s="6">
         <f t="shared" si="14"/>
-        <v>2.4472499999999999</v>
-      </c>
-      <c r="T17" s="20" t="s">
+        <v>2.5310833333333331</v>
+      </c>
+      <c r="T17" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C18">
@@ -1884,73 +1872,138 @@
         <v>2.546416666666667</v>
       </c>
     </row>
-    <row r="19" ht="14.25">
-      <c r="F19" s="4">
+    <row r="19" s="6" customFormat="1" ht="14.25">
+      <c r="A19" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="6">
+        <v>2.23</v>
+      </c>
+      <c r="D19" s="6">
+        <v>3.9700000000000002</v>
+      </c>
+      <c r="E19" s="6">
+        <v>3.6760000000000002</v>
+      </c>
+      <c r="F19" s="8">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="3" t="e">
+        <v>0.29400000000000004</v>
+      </c>
+      <c r="G19" s="9">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" t="e">
+        <v>13.183856502242156</v>
+      </c>
+      <c r="H19" s="6">
+        <v>3</v>
+      </c>
+      <c r="I19" s="6">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M19" s="5"/>
+        <v>0.098000000000000018</v>
+      </c>
+      <c r="J19" s="6">
+        <v>1</v>
+      </c>
+      <c r="K19" s="6">
+        <v>1</v>
+      </c>
+      <c r="L19" s="6">
+        <v>2</v>
+      </c>
+      <c r="M19" s="10">
+        <v>50000</v>
+      </c>
+      <c r="N19" s="10">
+        <v>50000</v>
+      </c>
       <c r="O19" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="6" t="e">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="P19" s="6">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0.098000000000000045</v>
       </c>
       <c r="Q19" s="9">
         <f t="shared" si="12"/>
-        <v>-1</v>
-      </c>
-      <c r="R19" s="6" t="e">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R19" s="6">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S19" t="e">
+        <v>2.2463333333333333</v>
+      </c>
+      <c r="S19" s="6">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" ht="14.25">
-      <c r="F20" s="4">
+        <v>2.3443333333333332</v>
+      </c>
+    </row>
+    <row r="20" s="6" customFormat="1" ht="14.25">
+      <c r="A20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1.6699999999999999</v>
+      </c>
+      <c r="D20" s="6">
+        <v>3.8660000000000001</v>
+      </c>
+      <c r="E20" s="6">
+        <v>3.4969999999999999</v>
+      </c>
+      <c r="F20" s="8">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="3" t="e">
+        <v>0.36900000000000022</v>
+      </c>
+      <c r="G20" s="9">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I20" t="e">
+        <v>22.095808383233546</v>
+      </c>
+      <c r="H20" s="6">
+        <v>2</v>
+      </c>
+      <c r="I20" s="6">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>0.18450000000000011</v>
+      </c>
+      <c r="J20" s="6">
+        <v>1</v>
+      </c>
+      <c r="K20" s="6">
+        <v>1</v>
+      </c>
+      <c r="L20" s="6">
+        <v>2</v>
+      </c>
+      <c r="M20" s="10">
+        <v>50000</v>
+      </c>
+      <c r="N20" s="10">
+        <v>100000</v>
       </c>
       <c r="O20" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="6" t="e">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="P20" s="6">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0.21525000000000014</v>
       </c>
       <c r="Q20" s="9">
         <f t="shared" si="12"/>
-        <v>-1</v>
-      </c>
-      <c r="R20" s="6" t="e">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R20" s="6">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S20" t="e">
+        <v>1.70075</v>
+      </c>
+      <c r="S20" s="6">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>1.9160000000000001</v>
       </c>
     </row>
     <row r="21" ht="14.25">
@@ -2162,7 +2215,7 @@
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>47</v>
@@ -2229,12 +2282,12 @@
         <v>2.9570833333333337</v>
       </c>
       <c r="T27" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>19</v>
@@ -2300,12 +2353,12 @@
         <v>1.6583341499999997</v>
       </c>
       <c r="T28" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>47</v>
@@ -2371,12 +2424,12 @@
         <v>2.4300008499999999</v>
       </c>
       <c r="T29" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>47</v>
@@ -2442,7 +2495,7 @@
         <v>3.4110008499999998</v>
       </c>
       <c r="T30" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" ht="14.25">
@@ -2475,12 +2528,12 @@
     </row>
     <row r="34" ht="14.25">
       <c r="I34" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" ht="14.25">
       <c r="I35" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" ht="14.25"/>

</xml_diff>

<commit_message>
Organized Data Repo a bit better, Edits to some checks for tracking in tethered case
</commit_message>
<xml_diff>
--- a/FatMothSet1Guide.xlsx
+++ b/FatMothSet1Guide.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
   <extLst>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -181,6 +181,27 @@
     <t xml:space="preserve">Male </t>
   </si>
   <si>
+    <t>2025_09_19</t>
+  </si>
+  <si>
+    <t>2025_10_10</t>
+  </si>
+  <si>
+    <t>2025_10_13</t>
+  </si>
+  <si>
+    <t>2025_10_14</t>
+  </si>
+  <si>
+    <t>2025_10_16</t>
+  </si>
+  <si>
+    <t>2025_10_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check 1104</t>
+  </si>
+  <si>
     <t>2024_08_01</t>
   </si>
   <si>
@@ -197,12 +218,6 @@
   </si>
   <si>
     <t>2024_06_24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">check 1104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">check 1120 </t>
   </si>
 </sst>
 </file>
@@ -267,7 +282,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -326,6 +341,9 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
@@ -1317,19 +1335,19 @@
         <v>1.6666699999999999</v>
       </c>
       <c r="P10" s="6">
-        <f t="shared" ref="P10:P30" si="11">O10*I10</f>
+        <f t="shared" ref="P10:P26" si="11">O10*I10</f>
         <v>0.32166730999999987</v>
       </c>
       <c r="Q10" s="9">
-        <f t="shared" ref="Q10:Q30" si="12">K10-1+(M10/(3*10^5))</f>
+        <f t="shared" ref="Q10:Q26" si="12">K10-1+(M10/(3*10^5))</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="R10" s="6">
-        <f t="shared" ref="R10:R30" si="13">C10+(Q10*I10)</f>
+        <f t="shared" ref="R10:R26" si="13">C10+(Q10*I10)</f>
         <v>2.0473333333333334</v>
       </c>
       <c r="S10" s="6">
-        <f t="shared" ref="S10:S30" si="14">R10+(O10*I10)</f>
+        <f t="shared" ref="S10:S26" si="14">R10+(O10*I10)</f>
         <v>2.3690006433333335</v>
       </c>
       <c r="T10" s="6" t="s">
@@ -2007,496 +2025,422 @@
       </c>
     </row>
     <row r="21" ht="14.25">
+      <c r="A21" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21">
+        <v>1.9099999999999999</v>
+      </c>
+      <c r="D21">
+        <v>3.8260000000000001</v>
+      </c>
+      <c r="E21">
+        <v>3.4630000000000001</v>
+      </c>
       <c r="F21" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="3" t="e">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="G21" s="3">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I21" t="e">
+        <v>19.005235602094242</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>0.072599999999999998</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>5</v>
+      </c>
+      <c r="M21" s="5">
+        <v>100000</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
       </c>
       <c r="O21" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="6" t="e">
+        <v>3.6666699999999999</v>
+      </c>
+      <c r="P21" s="6">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0.26620024199999998</v>
       </c>
       <c r="Q21" s="9">
         <f t="shared" si="12"/>
-        <v>-1</v>
-      </c>
-      <c r="R21" s="6" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="R21" s="6">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S21" t="e">
+        <v>1.9341999999999999</v>
+      </c>
+      <c r="S21">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>2.2004002419999997</v>
       </c>
     </row>
     <row r="22" ht="14.25">
+      <c r="A22" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22">
+        <v>2.1779999999999999</v>
+      </c>
+      <c r="D22">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="E22">
+        <v>3.335</v>
+      </c>
       <c r="F22" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="3" t="e">
+        <v>0.81500000000000039</v>
+      </c>
+      <c r="G22" s="3">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I22" t="e">
+        <v>37.419651056014715</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>0.2037500000000001</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>3</v>
+      </c>
+      <c r="M22" s="5">
+        <v>100000</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
       </c>
       <c r="O22" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="6" t="e">
+        <v>1.6666699999999999</v>
+      </c>
+      <c r="P22" s="6">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0.33958401250000014</v>
       </c>
       <c r="Q22" s="9">
         <f t="shared" si="12"/>
-        <v>-1</v>
-      </c>
-      <c r="R22" s="6" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="R22" s="6">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S22" t="e">
+        <v>2.2459166666666666</v>
+      </c>
+      <c r="S22">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>2.5855006791666666</v>
       </c>
     </row>
     <row r="23" ht="14.25">
+      <c r="A23" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23">
+        <v>1.782</v>
+      </c>
+      <c r="D23">
+        <v>4.306</v>
+      </c>
+      <c r="E23">
+        <v>3.8109999999999999</v>
+      </c>
       <c r="F23" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="3" t="e">
+        <v>0.49500000000000011</v>
+      </c>
+      <c r="G23" s="3">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I23" t="e">
+        <v>27.777777777777786</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>0.16500000000000004</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23" s="5">
+        <v>100000</v>
       </c>
       <c r="O23" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P23" s="6" t="e">
+        <v>1.3333299999999999</v>
+      </c>
+      <c r="P23" s="6">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0.21999945000000004</v>
       </c>
       <c r="Q23" s="9">
         <f t="shared" si="12"/>
-        <v>-1</v>
-      </c>
-      <c r="R23" s="6" t="e">
+        <v>3.3333333333333333e-06</v>
+      </c>
+      <c r="R23" s="6">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S23" t="e">
+        <v>1.78200055</v>
+      </c>
+      <c r="S23">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>2.0020000000000002</v>
       </c>
     </row>
     <row r="24" ht="14.25">
+      <c r="A24" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24">
+        <v>1.4239999999999999</v>
+      </c>
+      <c r="D24">
+        <v>4.5650000000000004</v>
+      </c>
+      <c r="E24">
+        <v>4.2770000000000001</v>
+      </c>
       <c r="F24" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="3" t="e">
+        <v>0.28800000000000026</v>
+      </c>
+      <c r="G24" s="3">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I24" t="e">
+        <v>20.224719101123615</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J24" s="1"/>
+        <v>0.072000000000000064</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>3</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24" s="5">
+        <v>100000</v>
+      </c>
       <c r="O24" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P24" s="6" t="e">
+        <v>2.3333300000000001</v>
+      </c>
+      <c r="P24" s="6">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0.16799976000000016</v>
       </c>
       <c r="Q24" s="9">
         <f t="shared" si="12"/>
-        <v>-1</v>
-      </c>
-      <c r="R24" s="6" t="e">
+        <v>3.3333333333333333e-06</v>
+      </c>
+      <c r="R24" s="6">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S24" t="e">
+        <v>1.42400024</v>
+      </c>
+      <c r="S24">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>1.5920000000000001</v>
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="D25" s="1"/>
+      <c r="A25" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25">
+        <v>2.2370000000000001</v>
+      </c>
+      <c r="D25" s="1">
+        <v>4.516</v>
+      </c>
+      <c r="E25">
+        <v>3.8999999999999999</v>
+      </c>
       <c r="F25" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="3" t="e">
+        <v>0.6160000000000001</v>
+      </c>
+      <c r="G25" s="3">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I25" t="e">
+        <v>27.536879749664735</v>
+      </c>
+      <c r="H25">
+        <v>5</v>
+      </c>
+      <c r="I25">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>0.12320000000000002</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>5</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25" s="5">
+        <v>200000</v>
       </c>
       <c r="O25" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="6" t="e">
+        <v>4.6666633333333332</v>
+      </c>
+      <c r="P25" s="6">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0.57493292266666673</v>
       </c>
       <c r="Q25" s="9">
         <f t="shared" si="12"/>
-        <v>-1</v>
-      </c>
-      <c r="R25" s="6" t="e">
+        <v>3.3333333333333333e-06</v>
+      </c>
+      <c r="R25" s="6">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S25" t="e">
+        <v>2.2370004106666665</v>
+      </c>
+      <c r="S25">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>2.8119333333333332</v>
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="D26" s="1"/>
+      <c r="A26" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26">
+        <v>1.542</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4.5119999999999996</v>
+      </c>
+      <c r="E26">
+        <v>3.9529999999999998</v>
+      </c>
       <c r="F26" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="3" t="e">
+        <v>0.55899999999999972</v>
+      </c>
+      <c r="G26" s="3">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I26" t="e">
+        <v>36.251621271076509</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>0.13974999999999993</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <v>3</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26" s="5">
+        <v>150000</v>
       </c>
       <c r="O26" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P26" s="6" t="e">
+        <v>1.4999966666666666</v>
+      </c>
+      <c r="P26" s="6">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0.20962453416666657</v>
       </c>
       <c r="Q26" s="9">
         <f t="shared" si="12"/>
-        <v>-1</v>
-      </c>
-      <c r="R26" s="6" t="e">
+        <v>1.0000033333333334</v>
+      </c>
+      <c r="R26" s="6">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S26" t="e">
+        <v>1.6817504658333333</v>
+      </c>
+      <c r="S26">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>1.8913749999999998</v>
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27">
-        <v>2.6800000000000002</v>
-      </c>
-      <c r="D27" s="1">
-        <v>4.1699999999999999</v>
-      </c>
-      <c r="E27">
-        <v>3.8199999999999998</v>
-      </c>
-      <c r="F27" s="4">
-        <f t="shared" si="7"/>
-        <v>0.35000000000000009</v>
-      </c>
-      <c r="G27" s="3">
-        <f t="shared" si="8"/>
-        <v>13.059701492537314</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="9"/>
-        <v>0.35000000000000009</v>
-      </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27">
-        <v>1</v>
-      </c>
-      <c r="M27">
-        <f>1*10^5</f>
-        <v>100000</v>
-      </c>
-      <c r="N27">
-        <f>3.75*10^5</f>
-        <v>375000</v>
-      </c>
-      <c r="O27" s="6">
-        <f t="shared" ref="O27:O30" si="15">(L27+((N27+(5*10^4))/(6*10^5))-(K27+((M27+(5*10^4))/(6*10^5))))</f>
-        <v>0.45833333333333348</v>
-      </c>
-      <c r="P27" s="6">
-        <f t="shared" si="11"/>
-        <v>0.16041666666666676</v>
-      </c>
-      <c r="Q27" s="9">
-        <f t="shared" si="12"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="R27" s="6">
-        <f t="shared" si="13"/>
-        <v>2.7966666666666669</v>
-      </c>
-      <c r="S27">
-        <f t="shared" si="14"/>
-        <v>2.9570833333333337</v>
-      </c>
-      <c r="T27" t="s">
-        <v>55</v>
-      </c>
+      <c r="F27"/>
+      <c r="G27"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28">
-        <v>1.25</v>
-      </c>
-      <c r="D28">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="E28">
-        <v>3.8599999999999999</v>
-      </c>
-      <c r="F28" s="4">
-        <f t="shared" si="7"/>
-        <v>0.48999999999999977</v>
-      </c>
-      <c r="G28" s="3">
-        <f t="shared" si="8"/>
-        <v>39.199999999999982</v>
-      </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="9"/>
-        <v>0.48999999999999977</v>
-      </c>
-      <c r="J28">
-        <v>1</v>
-      </c>
-      <c r="K28">
-        <v>1</v>
-      </c>
-      <c r="L28">
-        <v>1</v>
-      </c>
-      <c r="M28">
-        <v>1</v>
-      </c>
-      <c r="N28">
-        <f>5*10^5</f>
-        <v>500000</v>
-      </c>
-      <c r="O28" s="6">
-        <f t="shared" si="15"/>
-        <v>0.83333166666666658</v>
-      </c>
-      <c r="P28" s="6">
-        <f t="shared" si="11"/>
-        <v>0.40833251666666642</v>
-      </c>
-      <c r="Q28" s="9">
-        <f t="shared" si="12"/>
-        <v>3.3333333333333333e-06</v>
-      </c>
-      <c r="R28" s="6">
-        <f t="shared" si="13"/>
-        <v>1.2500016333333333</v>
-      </c>
-      <c r="S28">
-        <f t="shared" si="14"/>
-        <v>1.6583341499999997</v>
-      </c>
-      <c r="T28" t="s">
-        <v>55</v>
-      </c>
+      <c r="F28"/>
+      <c r="G28"/>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29">
-        <v>2.0899999999999999</v>
-      </c>
-      <c r="D29">
-        <v>3.96</v>
-      </c>
-      <c r="E29">
-        <v>3.4500000000000002</v>
-      </c>
-      <c r="F29" s="4">
-        <f t="shared" si="7"/>
-        <v>0.50999999999999979</v>
-      </c>
-      <c r="G29" s="3">
-        <f t="shared" si="8"/>
-        <v>24.401913875598076</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="9"/>
-        <v>0.50999999999999979</v>
-      </c>
-      <c r="J29">
-        <v>1</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="L29">
-        <v>1</v>
-      </c>
-      <c r="M29">
-        <v>1</v>
-      </c>
-      <c r="N29">
-        <f>4*10^5</f>
-        <v>400000</v>
-      </c>
-      <c r="O29" s="6">
-        <f t="shared" si="15"/>
-        <v>0.66666500000000006</v>
-      </c>
-      <c r="P29" s="6">
-        <f t="shared" si="11"/>
-        <v>0.33999914999999992</v>
-      </c>
-      <c r="Q29" s="9">
-        <f t="shared" si="12"/>
-        <v>3.3333333333333333e-06</v>
-      </c>
-      <c r="R29" s="6">
-        <f t="shared" si="13"/>
-        <v>2.0900016999999997</v>
-      </c>
-      <c r="S29">
-        <f t="shared" si="14"/>
-        <v>2.4300008499999999</v>
-      </c>
-      <c r="T29" t="s">
-        <v>58</v>
-      </c>
+      <c r="F29"/>
+      <c r="G29"/>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30">
-        <v>3.02</v>
-      </c>
-      <c r="D30">
-        <v>4.4299999999999997</v>
-      </c>
-      <c r="E30">
-        <v>3.9199999999999999</v>
-      </c>
-      <c r="F30" s="4">
-        <f t="shared" si="7"/>
-        <v>0.50999999999999979</v>
-      </c>
-      <c r="G30" s="3">
-        <f t="shared" si="8"/>
-        <v>16.887417218543039</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="9"/>
-        <v>0.50999999999999979</v>
-      </c>
-      <c r="J30">
-        <v>1</v>
-      </c>
-      <c r="K30">
-        <v>1</v>
-      </c>
-      <c r="L30">
-        <v>1</v>
-      </c>
-      <c r="M30">
-        <v>1</v>
-      </c>
-      <c r="N30">
-        <f>4.6*10^5</f>
-        <v>459999.99999999994</v>
-      </c>
-      <c r="O30" s="6">
-        <f t="shared" si="15"/>
-        <v>0.76666499999999993</v>
-      </c>
-      <c r="P30" s="6">
-        <f t="shared" si="11"/>
-        <v>0.3909991499999998</v>
-      </c>
-      <c r="Q30" s="9">
-        <f t="shared" si="12"/>
-        <v>3.3333333333333333e-06</v>
-      </c>
-      <c r="R30" s="6">
-        <f t="shared" si="13"/>
-        <v>3.0200016999999999</v>
-      </c>
-      <c r="S30">
-        <f t="shared" si="14"/>
-        <v>3.4110008499999998</v>
-      </c>
-      <c r="T30" t="s">
-        <v>58</v>
-      </c>
+      <c r="F30"/>
+      <c r="G30"/>
     </row>
     <row r="31" ht="14.25">
       <c r="F31" s="4">
@@ -2532,13 +2476,290 @@
       </c>
     </row>
     <row r="35" ht="14.25">
-      <c r="I35" t="s">
+      <c r="A35" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="36" ht="14.25"/>
-    <row r="37" ht="14.25"/>
-    <row r="38" ht="14.25"/>
+      <c r="B35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35">
+        <v>2.6800000000000002</v>
+      </c>
+      <c r="D35" s="1">
+        <v>4.1699999999999999</v>
+      </c>
+      <c r="E35">
+        <v>3.8199999999999998</v>
+      </c>
+      <c r="F35" s="4">
+        <f>D35-E35</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="G35" s="3">
+        <f>F35/C35*100</f>
+        <v>13.059701492537314</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <f>F35/H35</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <f>1*10^5</f>
+        <v>100000</v>
+      </c>
+      <c r="N35">
+        <f>3.75*10^5</f>
+        <v>375000</v>
+      </c>
+      <c r="O35" s="6">
+        <f>(L35+((N35+(5*10^4))/(6*10^5))-(K35+((M35+(5*10^4))/(6*10^5))))</f>
+        <v>0.45833333333333348</v>
+      </c>
+      <c r="P35" s="6">
+        <f>O35*I35</f>
+        <v>0.16041666666666676</v>
+      </c>
+      <c r="Q35" s="9">
+        <f>K35-1+(M35/(3*10^5))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="R35" s="6">
+        <f>C35+(Q35*I35)</f>
+        <v>2.7966666666666669</v>
+      </c>
+      <c r="S35">
+        <f>R35+(O35*I35)</f>
+        <v>2.9570833333333337</v>
+      </c>
+      <c r="T35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36">
+        <v>1.25</v>
+      </c>
+      <c r="D36">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="E36">
+        <v>3.8599999999999999</v>
+      </c>
+      <c r="F36" s="4">
+        <f>D36-E36</f>
+        <v>0.48999999999999977</v>
+      </c>
+      <c r="G36" s="3">
+        <f>F36/C36*100</f>
+        <v>39.199999999999982</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <f>F36/H36</f>
+        <v>0.48999999999999977</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <f>5*10^5</f>
+        <v>500000</v>
+      </c>
+      <c r="O36" s="6">
+        <f>(L36+((N36+(5*10^4))/(6*10^5))-(K36+((M36+(5*10^4))/(6*10^5))))</f>
+        <v>0.83333166666666658</v>
+      </c>
+      <c r="P36" s="6">
+        <f>O36*I36</f>
+        <v>0.40833251666666642</v>
+      </c>
+      <c r="Q36" s="9">
+        <f>K36-1+(M36/(3*10^5))</f>
+        <v>3.3333333333333333e-06</v>
+      </c>
+      <c r="R36" s="6">
+        <f>C36+(Q36*I36)</f>
+        <v>1.2500016333333333</v>
+      </c>
+      <c r="S36">
+        <f>R36+(O36*I36)</f>
+        <v>1.6583341499999997</v>
+      </c>
+      <c r="T36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="A37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37">
+        <v>2.0899999999999999</v>
+      </c>
+      <c r="D37">
+        <v>3.96</v>
+      </c>
+      <c r="E37">
+        <v>3.4500000000000002</v>
+      </c>
+      <c r="F37" s="4">
+        <f>D37-E37</f>
+        <v>0.50999999999999979</v>
+      </c>
+      <c r="G37" s="3">
+        <f>F37/C37*100</f>
+        <v>24.401913875598076</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <f>F37/H37</f>
+        <v>0.50999999999999979</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <f>4*10^5</f>
+        <v>400000</v>
+      </c>
+      <c r="O37" s="6">
+        <f>(L37+((N37+(5*10^4))/(6*10^5))-(K37+((M37+(5*10^4))/(6*10^5))))</f>
+        <v>0.66666500000000006</v>
+      </c>
+      <c r="P37" s="6">
+        <f>O37*I37</f>
+        <v>0.33999914999999992</v>
+      </c>
+      <c r="Q37" s="9">
+        <f>K37-1+(M37/(3*10^5))</f>
+        <v>3.3333333333333333e-06</v>
+      </c>
+      <c r="R37" s="6">
+        <f>C37+(Q37*I37)</f>
+        <v>2.0900016999999997</v>
+      </c>
+      <c r="S37">
+        <f>R37+(O37*I37)</f>
+        <v>2.4300008499999999</v>
+      </c>
+      <c r="T37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38">
+        <v>3.02</v>
+      </c>
+      <c r="D38">
+        <v>4.4299999999999997</v>
+      </c>
+      <c r="E38">
+        <v>3.9199999999999999</v>
+      </c>
+      <c r="F38" s="4">
+        <f>D38-E38</f>
+        <v>0.50999999999999979</v>
+      </c>
+      <c r="G38" s="3">
+        <f>F38/C38*100</f>
+        <v>16.887417218543039</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <f>F38/H38</f>
+        <v>0.50999999999999979</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <f>4.6*10^5</f>
+        <v>459999.99999999994</v>
+      </c>
+      <c r="O38" s="6">
+        <f>(L38+((N38+(5*10^4))/(6*10^5))-(K38+((M38+(5*10^4))/(6*10^5))))</f>
+        <v>0.76666499999999993</v>
+      </c>
+      <c r="P38" s="6">
+        <f>O38*I38</f>
+        <v>0.3909991499999998</v>
+      </c>
+      <c r="Q38" s="9">
+        <f>K38-1+(M38/(3*10^5))</f>
+        <v>3.3333333333333333e-06</v>
+      </c>
+      <c r="R38" s="6">
+        <f>C38+(Q38*I38)</f>
+        <v>3.0200016999999999</v>
+      </c>
+      <c r="S38">
+        <f>R38+(O38*I38)</f>
+        <v>3.4110008499999998</v>
+      </c>
+      <c r="T38" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="39" ht="14.25"/>
     <row r="40" ht="14.25"/>
     <row r="45" ht="14.25"/>

</xml_diff>